<commit_message>
Create django back (base)
</commit_message>
<xml_diff>
--- a/Documentation/Planification.xlsx
+++ b/Documentation/Planification.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alan.chambaz\Desktop\HES\CloudStation\HES\3ème\Dev Web\Projet Django\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\DW-WTM-Git\Wolves-Tournament-Master\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CC08E7-A02D-4838-B0B8-D474A3471A9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B9C7B4-25C5-4C1E-89C2-9C3B03FDDB81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{86F466E6-282D-47AC-8147-7CB72DB0041F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="57">
   <si>
     <t>Tâche</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>Page de gestion de notifications (connected user)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Déploiement</t>
   </si>
 </sst>
 </file>
@@ -244,7 +247,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,6 +299,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -375,7 +384,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -455,18 +464,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -479,6 +476,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,11 +812,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{817B9D33-C5B8-4FAA-9ED6-20225FB0C8F1}">
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+      <pane ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -825,21 +837,21 @@
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="29" t="s">
+      <c r="E2" s="37"/>
+      <c r="F2" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="32" t="s">
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
@@ -888,8 +900,8 @@
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
       <c r="F4" s="21"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="33"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="29"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="19"/>
@@ -908,8 +920,8 @@
       <c r="D5" s="10"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="33"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="29"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="19"/>
@@ -928,8 +940,8 @@
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="33"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="29"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
@@ -948,8 +960,8 @@
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="33"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="29"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="19"/>
@@ -978,7 +990,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="22"/>
-      <c r="G9" s="34"/>
+      <c r="G9" s="30"/>
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
       <c r="J9" s="22"/>
@@ -998,7 +1010,7 @@
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="22"/>
-      <c r="G10" s="34"/>
+      <c r="G10" s="30"/>
       <c r="H10" s="22"/>
       <c r="I10" s="24"/>
       <c r="J10" s="22"/>
@@ -1018,7 +1030,7 @@
       <c r="D11" s="12"/>
       <c r="E11" s="8"/>
       <c r="F11" s="22"/>
-      <c r="G11" s="34"/>
+      <c r="G11" s="30"/>
       <c r="H11" s="22"/>
       <c r="I11" s="22"/>
       <c r="J11" s="22"/>
@@ -1038,12 +1050,12 @@
       <c r="D12" s="9"/>
       <c r="E12" s="12"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="34"/>
+      <c r="G12" s="30"/>
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
-      <c r="J12" s="35"/>
+      <c r="J12" s="31"/>
       <c r="K12" s="19"/>
-      <c r="L12" s="35"/>
+      <c r="L12" s="31"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
@@ -1056,12 +1068,12 @@
       <c r="D13" s="9"/>
       <c r="E13" s="8"/>
       <c r="F13" s="22"/>
-      <c r="G13" s="34"/>
+      <c r="G13" s="30"/>
       <c r="H13" s="22"/>
       <c r="I13" s="22"/>
-      <c r="J13" s="35"/>
+      <c r="J13" s="31"/>
       <c r="K13" s="19"/>
-      <c r="L13" s="35"/>
+      <c r="L13" s="31"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
@@ -1084,14 +1096,14 @@
       <c r="B15" s="9"/>
       <c r="C15" s="18"/>
       <c r="D15" s="22"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="36"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="32"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
@@ -1106,7 +1118,7 @@
       <c r="D16" s="22"/>
       <c r="E16" s="23"/>
       <c r="F16" s="22"/>
-      <c r="G16" s="34"/>
+      <c r="G16" s="30"/>
       <c r="H16" s="22"/>
       <c r="I16" s="22"/>
       <c r="J16" s="22"/>
@@ -1122,7 +1134,7 @@
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
-      <c r="G17" s="34"/>
+      <c r="G17" s="30"/>
       <c r="H17" s="22"/>
       <c r="I17" s="22"/>
       <c r="J17" s="22"/>
@@ -1140,7 +1152,7 @@
       <c r="D18" s="22"/>
       <c r="E18" s="23"/>
       <c r="F18" s="23"/>
-      <c r="G18" s="34"/>
+      <c r="G18" s="30"/>
       <c r="H18" s="22"/>
       <c r="I18" s="22"/>
       <c r="J18" s="22"/>
@@ -1154,7 +1166,7 @@
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
-      <c r="G19" s="34"/>
+      <c r="G19" s="30"/>
       <c r="H19" s="22"/>
       <c r="I19" s="22"/>
       <c r="J19" s="22"/>
@@ -1170,7 +1182,7 @@
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
-      <c r="G20" s="34"/>
+      <c r="G20" s="30"/>
       <c r="H20" s="22"/>
       <c r="I20" s="22"/>
       <c r="J20" s="22"/>
@@ -1188,7 +1200,7 @@
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
       <c r="F21" s="23"/>
-      <c r="G21" s="38"/>
+      <c r="G21" s="34"/>
       <c r="H21" s="22"/>
       <c r="I21" s="22"/>
       <c r="J21" s="22"/>
@@ -1206,7 +1218,7 @@
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
       <c r="F22" s="23"/>
-      <c r="G22" s="38"/>
+      <c r="G22" s="34"/>
       <c r="H22" s="22"/>
       <c r="I22" s="22"/>
       <c r="J22" s="22"/>
@@ -1224,7 +1236,7 @@
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
       <c r="F23" s="23"/>
-      <c r="G23" s="38"/>
+      <c r="G23" s="34"/>
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
       <c r="J23" s="22"/>
@@ -1242,7 +1254,7 @@
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
       <c r="F24" s="23"/>
-      <c r="G24" s="38"/>
+      <c r="G24" s="34"/>
       <c r="H24" s="22"/>
       <c r="I24" s="22"/>
       <c r="J24" s="22"/>
@@ -1260,7 +1272,7 @@
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
-      <c r="G25" s="34"/>
+      <c r="G25" s="30"/>
       <c r="H25" s="22"/>
       <c r="I25" s="23"/>
       <c r="J25" s="23"/>
@@ -1274,7 +1286,7 @@
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
-      <c r="G26" s="34"/>
+      <c r="G26" s="30"/>
       <c r="H26" s="22"/>
       <c r="I26" s="22"/>
       <c r="J26" s="22"/>
@@ -1290,7 +1302,7 @@
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
-      <c r="G27" s="34"/>
+      <c r="G27" s="30"/>
       <c r="H27" s="22"/>
       <c r="I27" s="22"/>
       <c r="J27" s="22"/>
@@ -1308,7 +1320,7 @@
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
-      <c r="G28" s="38"/>
+      <c r="G28" s="34"/>
       <c r="H28" s="23"/>
       <c r="I28" s="23"/>
       <c r="J28" s="23"/>
@@ -1322,7 +1334,7 @@
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
-      <c r="G29" s="34"/>
+      <c r="G29" s="30"/>
       <c r="H29" s="22"/>
       <c r="I29" s="22"/>
       <c r="J29" s="22"/>
@@ -1338,7 +1350,7 @@
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
-      <c r="G30" s="34"/>
+      <c r="G30" s="30"/>
       <c r="H30" s="22"/>
       <c r="I30" s="22"/>
       <c r="J30" s="22"/>
@@ -1356,7 +1368,7 @@
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
       <c r="F31" s="23"/>
-      <c r="G31" s="38"/>
+      <c r="G31" s="34"/>
       <c r="H31" s="22"/>
       <c r="I31" s="22"/>
       <c r="J31" s="22"/>
@@ -1374,12 +1386,12 @@
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
-      <c r="G32" s="38"/>
+      <c r="G32" s="34"/>
       <c r="H32" s="23"/>
       <c r="I32" s="22"/>
       <c r="J32" s="22"/>
       <c r="K32" s="19"/>
-      <c r="L32" s="34"/>
+      <c r="L32" s="30"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
@@ -1392,7 +1404,7 @@
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
       <c r="F33" s="22"/>
-      <c r="G33" s="34"/>
+      <c r="G33" s="30"/>
       <c r="H33" s="23"/>
       <c r="I33" s="22"/>
       <c r="J33" s="22"/>
@@ -1410,7 +1422,7 @@
       <c r="D34" s="22"/>
       <c r="E34" s="22"/>
       <c r="F34" s="22"/>
-      <c r="G34" s="34"/>
+      <c r="G34" s="30"/>
       <c r="H34" s="23"/>
       <c r="I34" s="22"/>
       <c r="J34" s="22"/>
@@ -1428,7 +1440,7 @@
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
       <c r="F35" s="22"/>
-      <c r="G35" s="34"/>
+      <c r="G35" s="30"/>
       <c r="H35" s="22"/>
       <c r="I35" s="22"/>
       <c r="J35" s="23"/>
@@ -1446,7 +1458,7 @@
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
       <c r="F36" s="23"/>
-      <c r="G36" s="34"/>
+      <c r="G36" s="30"/>
       <c r="H36" s="22"/>
       <c r="I36" s="22"/>
       <c r="J36" s="22"/>
@@ -1464,7 +1476,7 @@
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
       <c r="F37" s="23"/>
-      <c r="G37" s="38"/>
+      <c r="G37" s="34"/>
       <c r="H37" s="22"/>
       <c r="I37" s="22"/>
       <c r="J37" s="22"/>
@@ -1476,13 +1488,13 @@
         <v>55</v>
       </c>
       <c r="B38" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="22"/>
       <c r="E38" s="22"/>
       <c r="F38" s="22"/>
-      <c r="G38" s="34"/>
+      <c r="G38" s="30"/>
       <c r="H38" s="22"/>
       <c r="I38" s="23"/>
       <c r="J38" s="22"/>
@@ -1496,7 +1508,7 @@
       <c r="D39" s="22"/>
       <c r="E39" s="22"/>
       <c r="F39" s="22"/>
-      <c r="G39" s="34"/>
+      <c r="G39" s="30"/>
       <c r="H39" s="22"/>
       <c r="I39" s="22"/>
       <c r="J39" s="22"/>
@@ -1514,7 +1526,7 @@
       <c r="D40" s="22"/>
       <c r="E40" s="22"/>
       <c r="F40" s="22"/>
-      <c r="G40" s="34"/>
+      <c r="G40" s="30"/>
       <c r="H40" s="22"/>
       <c r="I40" s="22"/>
       <c r="J40" s="22"/>
@@ -1528,7 +1540,7 @@
       <c r="D41" s="22"/>
       <c r="E41" s="22"/>
       <c r="F41" s="22"/>
-      <c r="G41" s="34"/>
+      <c r="G41" s="30"/>
       <c r="H41" s="22"/>
       <c r="I41" s="22"/>
       <c r="J41" s="22"/>
@@ -1544,7 +1556,7 @@
       <c r="D42" s="22"/>
       <c r="E42" s="22"/>
       <c r="F42" s="22"/>
-      <c r="G42" s="34"/>
+      <c r="G42" s="30"/>
       <c r="H42" s="22"/>
       <c r="I42" s="22"/>
       <c r="J42" s="22"/>
@@ -1562,7 +1574,7 @@
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
       <c r="F43" s="22"/>
-      <c r="G43" s="34"/>
+      <c r="G43" s="30"/>
       <c r="H43" s="22"/>
       <c r="I43" s="22"/>
       <c r="J43" s="22"/>
@@ -1580,7 +1592,7 @@
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
       <c r="F44" s="22"/>
-      <c r="G44" s="34"/>
+      <c r="G44" s="30"/>
       <c r="H44" s="22"/>
       <c r="I44" s="22"/>
       <c r="J44" s="22"/>
@@ -1594,7 +1606,7 @@
       <c r="D45" s="22"/>
       <c r="E45" s="22"/>
       <c r="F45" s="22"/>
-      <c r="G45" s="34"/>
+      <c r="G45" s="30"/>
       <c r="H45" s="22"/>
       <c r="I45" s="22"/>
       <c r="J45" s="22"/>
@@ -1603,32 +1615,30 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B46" s="9"/>
+        <v>56</v>
+      </c>
+      <c r="B46" s="9">
+        <v>1</v>
+      </c>
       <c r="C46" s="18"/>
       <c r="D46" s="22"/>
       <c r="E46" s="22"/>
-      <c r="F46" s="22"/>
-      <c r="G46" s="34"/>
+      <c r="F46" s="39"/>
+      <c r="G46" s="30"/>
       <c r="H46" s="22"/>
       <c r="I46" s="22"/>
       <c r="J46" s="22"/>
       <c r="K46" s="19"/>
-      <c r="L46" s="22"/>
+      <c r="L46" s="39"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A47" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B47" s="9">
-        <v>1</v>
-      </c>
+      <c r="A47" s="8"/>
+      <c r="B47" s="9"/>
       <c r="C47" s="18"/>
       <c r="D47" s="22"/>
       <c r="E47" s="22"/>
       <c r="F47" s="22"/>
-      <c r="G47" s="34"/>
+      <c r="G47" s="30"/>
       <c r="H47" s="22"/>
       <c r="I47" s="22"/>
       <c r="J47" s="22"/>
@@ -1636,17 +1646,15 @@
       <c r="L47" s="22"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B48" s="9">
-        <v>1</v>
-      </c>
+      <c r="A48" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" s="9"/>
       <c r="C48" s="18"/>
       <c r="D48" s="22"/>
       <c r="E48" s="22"/>
       <c r="F48" s="22"/>
-      <c r="G48" s="34"/>
+      <c r="G48" s="30"/>
       <c r="H48" s="22"/>
       <c r="I48" s="22"/>
       <c r="J48" s="22"/>
@@ -1655,7 +1663,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B49" s="9">
         <v>1</v>
@@ -1663,48 +1671,84 @@
       <c r="C49" s="18"/>
       <c r="D49" s="22"/>
       <c r="E49" s="22"/>
-      <c r="F49" s="35"/>
-      <c r="G49" s="34"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="30"/>
       <c r="H49" s="22"/>
       <c r="I49" s="22"/>
       <c r="J49" s="22"/>
       <c r="K49" s="19"/>
       <c r="L49" s="22"/>
     </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A50" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B50" s="9">
+        <v>1</v>
+      </c>
+      <c r="C50" s="18"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="30"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="22"/>
+      <c r="J50" s="22"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="22"/>
+    </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C51" t="s">
+      <c r="A51" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B51" s="9">
+        <v>1</v>
+      </c>
+      <c r="C51" s="18"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="31"/>
+      <c r="G51" s="30"/>
+      <c r="H51" s="22"/>
+      <c r="I51" s="22"/>
+      <c r="J51" s="22"/>
+      <c r="K51" s="19"/>
+      <c r="L51" s="22"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
         <v>16</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E53" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E52" t="s">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E54" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E53" t="s">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E55" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C55" t="s">
-        <v>24</v>
-      </c>
-      <c r="E55" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
+        <v>24</v>
+      </c>
+      <c r="E57" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
         <v>27</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D59" t="s">
         <v>26</v>
       </c>
-      <c r="E57" s="19"/>
+      <c r="E59" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>